<commit_message>
# more plant names in excel file + other script updates
</commit_message>
<xml_diff>
--- a/Data/new_sci_names_DOME_plants.xlsx
+++ b/Data/new_sci_names_DOME_plants.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgonzalez\Desktop\Dome\Dome_Invasion_Share\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28FE74A-B32D-4309-AD4F-107B2333C752}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF3FA5-3E7B-4CDD-9707-575DC03388D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{72953B1A-1545-4783-BD50-999F9166F3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,100 +31,381 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sitanion hystrix </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petalostemum candida </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hymenoxys argentea </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oryzopsis hymenoides </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oryzopsis micrantha </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>Bahia dissecta</t>
+  </si>
+  <si>
+    <t>Hymenothrix dissecta</t>
+  </si>
+  <si>
+    <t>Chenopodium graveolens</t>
+  </si>
+  <si>
+    <t>Dysphania graveolens</t>
+  </si>
+  <si>
+    <t>Chrysopsis villosa</t>
+  </si>
+  <si>
+    <t>Heterotheca villosa</t>
+  </si>
+  <si>
+    <t>Chrysothamnus nauseosus</t>
+  </si>
+  <si>
+    <t>Ericameria nauseosa</t>
+  </si>
+  <si>
+    <t>Cleome serrulata</t>
+  </si>
+  <si>
+    <t>Peritoma serrulate</t>
+  </si>
+  <si>
+    <t>Conyza canadensis</t>
+  </si>
+  <si>
+    <t>Erigeron canadensis</t>
+  </si>
+  <si>
+    <t>Cryptantha jamesii</t>
+  </si>
+  <si>
+    <t>Cryptantha cinerea</t>
+  </si>
+  <si>
+    <t>Euphorbia fendleri</t>
+  </si>
+  <si>
+    <t>Chamaesyce fendleri</t>
+  </si>
+  <si>
+    <t>Euphorbia revoluta</t>
+  </si>
+  <si>
+    <t>Chamaesyce revoluta</t>
   </si>
   <si>
     <t>Festuca octoflora</t>
   </si>
   <si>
-    <t xml:space="preserve">Chrysopsis villosa </t>
-  </si>
-  <si>
-    <t>Old</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Koeleria cristata </t>
+    <t>Vulpia octoflora</t>
+  </si>
+  <si>
+    <t>Gaura coccinea</t>
+  </si>
+  <si>
+    <t>Gaura suffrutescens</t>
+  </si>
+  <si>
+    <t>Haplopappus spinulosus</t>
+  </si>
+  <si>
+    <t>Xanthisma spinulosus</t>
+  </si>
+  <si>
+    <t>Hymenoxys argentea</t>
+  </si>
+  <si>
+    <t>Tetraneuris argentea</t>
+  </si>
+  <si>
+    <t>Koeleria cristata</t>
   </si>
   <si>
     <t>Koeleria macrantha</t>
   </si>
   <si>
+    <t>Laxx</t>
+  </si>
+  <si>
+    <t>Lappula occidentalis</t>
+  </si>
+  <si>
+    <t>Opuntia erinaceae</t>
+  </si>
+  <si>
+    <t>Opuntia polyacantha</t>
+  </si>
+  <si>
+    <t>Opuntia imbricata</t>
+  </si>
+  <si>
+    <t>Cylindropuntia imbricate</t>
+  </si>
+  <si>
+    <t>Oryzopsis hymenoides</t>
+  </si>
+  <si>
+    <t>Achnatherum hymenoides</t>
+  </si>
+  <si>
+    <t>Oryzopsis micrantha</t>
+  </si>
+  <si>
     <t>Piptatherum micranthum</t>
   </si>
   <si>
-    <t>Achnatherum hymenoides</t>
-  </si>
-  <si>
-    <t>Tetraneuris argentea</t>
-  </si>
-  <si>
-    <t>Heterotheca villosa</t>
+    <t>Petalostemum candida</t>
   </si>
   <si>
     <t>Dalea candida</t>
   </si>
   <si>
-    <t>Vulpia ocflora</t>
-  </si>
-  <si>
-    <t>Elymus ellymoides</t>
+    <t>Phxx</t>
+  </si>
+  <si>
+    <t>Phacelia heterophylla</t>
+  </si>
+  <si>
+    <t>Physalis foetens</t>
+  </si>
+  <si>
+    <t>Physalis subulate</t>
+  </si>
+  <si>
+    <t>Plantago purshii</t>
+  </si>
+  <si>
+    <t>Plantago patagonica</t>
+  </si>
+  <si>
+    <t>Salsola kali</t>
+  </si>
+  <si>
+    <t>Salsola tragus</t>
+  </si>
+  <si>
+    <t>Senecio multicapitatus</t>
+  </si>
+  <si>
+    <t>Senecio spartioides</t>
+  </si>
+  <si>
+    <t>Sisymbrium linearifolium</t>
+  </si>
+  <si>
+    <t>Hesperidanthus liniarifolius</t>
+  </si>
+  <si>
+    <t>Sitanion hystrix</t>
+  </si>
+  <si>
+    <t>Yucca angustissima</t>
+  </si>
+  <si>
+    <t>Yucca intermedia</t>
+  </si>
+  <si>
+    <t>Elymus elymoides</t>
   </si>
   <si>
     <t>new_code</t>
   </si>
   <si>
+    <t>hydi</t>
+  </si>
+  <si>
+    <t>dygr</t>
+  </si>
+  <si>
+    <t>hevi</t>
+  </si>
+  <si>
+    <t>erna</t>
+  </si>
+  <si>
+    <t>pese</t>
+  </si>
+  <si>
+    <t>erca</t>
+  </si>
+  <si>
+    <t>crci</t>
+  </si>
+  <si>
+    <t>chfe</t>
+  </si>
+  <si>
+    <t>chre</t>
+  </si>
+  <si>
+    <t>vuoc</t>
+  </si>
+  <si>
+    <t>gasu</t>
+  </si>
+  <si>
+    <t>xasp</t>
+  </si>
+  <si>
+    <t>tear</t>
+  </si>
+  <si>
+    <t>koma</t>
+  </si>
+  <si>
+    <t>laoc</t>
+  </si>
+  <si>
+    <t>oppo</t>
+  </si>
+  <si>
+    <t>cyim</t>
+  </si>
+  <si>
+    <t>achy</t>
+  </si>
+  <si>
+    <t>pimi</t>
+  </si>
+  <si>
+    <t>daca</t>
+  </si>
+  <si>
+    <t>phhe</t>
+  </si>
+  <si>
+    <t>phsu</t>
+  </si>
+  <si>
+    <t>plpa</t>
+  </si>
+  <si>
+    <t>satr</t>
+  </si>
+  <si>
+    <t>sesp</t>
+  </si>
+  <si>
+    <t>heli</t>
+  </si>
+  <si>
     <t>elel</t>
   </si>
   <si>
-    <t>vuoc</t>
-  </si>
-  <si>
-    <t>daca</t>
-  </si>
-  <si>
-    <t>hevi</t>
-  </si>
-  <si>
-    <t>tear</t>
-  </si>
-  <si>
-    <t>achy</t>
-  </si>
-  <si>
-    <t>pimi</t>
-  </si>
-  <si>
-    <t>koma</t>
+    <t>yuin</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>old_code</t>
+  </si>
+  <si>
+    <t>badi</t>
+  </si>
+  <si>
+    <t>chgr</t>
+  </si>
+  <si>
+    <t>chvi</t>
+  </si>
+  <si>
+    <t>chna</t>
+  </si>
+  <si>
+    <t>clse</t>
+  </si>
+  <si>
+    <t>coca</t>
+  </si>
+  <si>
+    <t>crja</t>
+  </si>
+  <si>
+    <t>eufe</t>
+  </si>
+  <si>
+    <t>eure</t>
+  </si>
+  <si>
+    <t>feoc</t>
+  </si>
+  <si>
+    <t>gaco</t>
+  </si>
+  <si>
+    <t>hasp</t>
+  </si>
+  <si>
+    <t>hyar</t>
+  </si>
+  <si>
+    <t>kocr</t>
+  </si>
+  <si>
+    <t>oper</t>
+  </si>
+  <si>
+    <t>opim</t>
+  </si>
+  <si>
+    <t>orhy</t>
+  </si>
+  <si>
+    <t>ormi</t>
+  </si>
+  <si>
+    <t>peca</t>
+  </si>
+  <si>
+    <t>phfo</t>
+  </si>
+  <si>
+    <t>plpu</t>
+  </si>
+  <si>
+    <t>saka</t>
+  </si>
+  <si>
+    <t>semu</t>
+  </si>
+  <si>
+    <t>sili</t>
+  </si>
+  <si>
+    <t>sihy</t>
+  </si>
+  <si>
+    <t>yuan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laxx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phxx </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF228622"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,8 +428,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,115 +746,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D63772-7022-4F62-907D-F76D3E96F5DF}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>